<commit_message>
Use --where option to filter models prior to export in dbt/scripts/export_models.py
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_neg_asmt_value.xlsx
+++ b/dbt/export/templates/qc.vw_report_neg_asmt_value.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2269EC8D-FB42-4BF1-9E35-8D4170703684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906AB859-15BD-4896-B455-119BDE0FFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{117FAC87-5613-4FBC-929F-755B4127EDFC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{117FAC87-5613-4FBC-929F-755B4127EDFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>PARID</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Class</t>
+  </si>
+  <si>
+    <t>TOWNSHIP</t>
   </si>
 </sst>
 </file>
@@ -642,230 +645,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C761DB-A6F0-4F3A-9C45-5D4B5AB4CC15}">
-  <dimension ref="A1:BO1"/>
+  <dimension ref="A1:BP1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="61" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="62" max="64" width="11" bestFit="1" customWidth="1"/>
-    <col min="65" max="67" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="70" max="92" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="93" max="129" width="21.5703125" customWidth="1"/>
-    <col min="130" max="132" width="24" bestFit="1" customWidth="1"/>
-    <col min="133" max="135" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="12" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="20" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="62" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="65" width="11" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="71" max="93" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="130" width="21.5703125" customWidth="1"/>
+    <col min="131" max="133" width="24" bestFit="1" customWidth="1"/>
+    <col min="134" max="136" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="12" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="20" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>